<commit_message>
SUPPORTED_MANIFESTS = +["blood_dna", "tissue_dna", "tumor_tissue_dna"]
</commit_message>
<xml_diff>
--- a/template_examples/tumor_tissue_DNA_template.xlsx
+++ b/template_examples/tumor_tissue_DNA_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFFAD44-BB0F-9F45-8BF8-3A1DCBC88A72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E76E75-1968-5A48-B185-115B65E67570}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="12460" windowWidth="33900" windowHeight="10580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,9 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1200,6 +1200,9 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1211,9 +1214,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1264,6 +1264,19 @@
       <sheetData sheetId="10"/>
       <sheetData sheetId="11"/>
       <sheetData sheetId="12"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Data Dictionary"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1592,8 +1605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F218"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1606,13 +1619,13 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" ht="17" thickBot="1">
       <c r="A2" t="s">
@@ -2851,7 +2864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AH202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
@@ -2884,42 +2897,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="15" customHeight="1">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="18" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="20"/>
-      <c r="Z1" s="17" t="s">
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="21"/>
+      <c r="Z1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="17"/>
-      <c r="AB1" s="17"/>
-      <c r="AC1" s="17"/>
-      <c r="AD1" s="17"/>
-      <c r="AE1" s="17"/>
-      <c r="AF1" s="17"/>
-      <c r="AG1" s="17"/>
-      <c r="AH1" s="17"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="18"/>
+      <c r="AG1" s="18"/>
+      <c r="AH1" s="18"/>
     </row>
     <row r="2" spans="1:34">
       <c r="A2" t="s">
@@ -2955,7 +2968,7 @@
       <c r="K2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="17" t="s">
         <v>116</v>
       </c>
       <c r="M2" s="2" t="s">

</xml_diff>